<commit_message>
I think we're good up to Turbidity
working on T-SSC plots now
</commit_message>
<xml_diff>
--- a/Data/Storm S table.xlsx
+++ b/Data/Storm S table.xlsx
@@ -434,7 +434,7 @@
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -512,10 +512,10 @@
         <v>40927.5625</v>
       </c>
       <c r="B2" t="n">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
         <v>0.0</v>
@@ -524,431 +524,431 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>304.7377240891975</v>
+        <v>578.0</v>
       </c>
       <c r="H2" t="n">
-        <v>304.7377240891975</v>
+        <v>578.0</v>
       </c>
       <c r="I2" t="n">
-        <v>258.65582999879837</v>
+        <v>291.08169999999996</v>
       </c>
       <c r="J2" t="n">
-        <v>1686552.7152968869</v>
+        <v>7634185.920000003</v>
       </c>
       <c r="K2" t="n">
-        <v>7809900.778202723</v>
+        <v>14665500.0</v>
       </c>
       <c r="L2" t="n">
-        <v>6123348.062905836</v>
+        <v>7031314.079999997</v>
       </c>
       <c r="M2" t="n">
-        <v>0.285</v>
+        <v>0.56</v>
       </c>
       <c r="N2" t="n">
         <v>1</v>
       </c>
       <c r="O2" t="n">
-        <v>0.326</v>
+        <v>0.606</v>
       </c>
       <c r="P2" t="n">
-        <v>0.04</v>
+        <v>0.046</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c s="2" r="A3" t="n">
-        <v>40941.260416666664</v>
+        <v>40933.15625</v>
       </c>
       <c r="B3" t="n">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D3" t="n">
-        <v>86.10196838196937</v>
+        <v>884.1915795502618</v>
       </c>
       <c r="E3" t="n">
-        <v>16.002</v>
+        <v>75.94600000000003</v>
       </c>
       <c r="F3" t="n">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="G3" t="n">
-        <v>286.4722882650073</v>
+        <v>1385.0</v>
       </c>
       <c r="H3" t="n">
-        <v>286.4722882650073</v>
+        <v>1385.0</v>
       </c>
       <c r="I3" t="n">
-        <v>202.20504562735888</v>
+        <v>810.124</v>
       </c>
       <c r="J3" t="n">
-        <v>2981915.66874523</v>
+        <v>10004715.612000002</v>
       </c>
       <c r="K3" t="n">
-        <v>10025065.005017411</v>
+        <v>23598000.0</v>
       </c>
       <c r="L3" t="n">
-        <v>7043149.336272181</v>
+        <v>13593284.387999998</v>
       </c>
       <c r="M3" t="n">
-        <v>0.529</v>
+        <v>0.171</v>
       </c>
       <c r="N3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O3" t="n">
-        <v>0.568</v>
+        <v>0.454</v>
       </c>
       <c r="P3" t="n">
-        <v>0.039</v>
+        <v>0.283</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c s="2" r="A4" t="n">
-        <v>40942.322916666664</v>
+        <v>40941.25</v>
       </c>
       <c r="B4" t="n">
         <v>95</v>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>121.89672415405421</v>
+        <v>85.18844701705477</v>
       </c>
       <c r="E4" t="n">
-        <v>14.731999999999998</v>
+        <v>16.002</v>
       </c>
       <c r="F4" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G4" t="n">
-        <v>361.9635596523701</v>
+        <v>525.0</v>
       </c>
       <c r="H4" t="n">
-        <v>361.9635596523701</v>
+        <v>525.0</v>
       </c>
       <c r="I4" t="n">
-        <v>298.0946270878208</v>
+        <v>229.1065</v>
       </c>
       <c r="J4" t="n">
-        <v>3021427.4556685165</v>
+        <v>10736915.13</v>
       </c>
       <c r="K4" t="n">
-        <v>12531913.846944192</v>
+        <v>19012500.0</v>
       </c>
       <c r="L4" t="n">
-        <v>9510486.391275676</v>
+        <v>8275584.869999999</v>
       </c>
       <c r="M4" t="n">
-        <v>1.064</v>
+        <v>1.004</v>
       </c>
       <c r="N4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O4" t="n">
-        <v>1.12</v>
+        <v>1.049</v>
       </c>
       <c r="P4" t="n">
-        <v>0.056</v>
+        <v>0.045</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c s="2" r="A5" t="n">
-        <v>40944.416666666664</v>
+        <v>40942.052083333336</v>
       </c>
       <c r="B5" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>136.1969361926139</v>
+        <v>52.76112169500943</v>
       </c>
       <c r="E5" t="n">
-        <v>19.050000000000004</v>
+        <v>9.144</v>
       </c>
       <c r="F5" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="G5" t="n">
-        <v>300.1327411547789</v>
+        <v>328.99999999999994</v>
       </c>
       <c r="H5" t="n">
-        <v>300.1327411547789</v>
+        <v>328.99999999999994</v>
       </c>
       <c r="I5" t="n">
-        <v>227.6553967836468</v>
+        <v>151.63750000000005</v>
       </c>
       <c r="J5" t="n">
-        <v>2652728.1170209795</v>
+        <v>2870346.2399999998</v>
       </c>
       <c r="K5" t="n">
-        <v>9748197.010306032</v>
+        <v>5136300.0</v>
       </c>
       <c r="L5" t="n">
-        <v>7095468.893285053</v>
+        <v>2265953.7600000002</v>
       </c>
       <c r="M5" t="n">
-        <v>0.498</v>
+        <v>0.148</v>
       </c>
       <c r="N5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O5" t="n">
-        <v>0.536</v>
+        <v>0.155</v>
       </c>
       <c r="P5" t="n">
-        <v>0.039</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c s="2" r="A6" t="n">
-        <v>40944.958333333336</v>
+        <v>40942.135416666664</v>
       </c>
       <c r="B6" t="n">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>170.9754430583344</v>
+        <v>21.270936482996685</v>
       </c>
       <c r="E6" t="n">
-        <v>78.48600000000002</v>
+        <v>6.096</v>
       </c>
       <c r="F6" t="n">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="G6" t="n">
-        <v>777.9615210634561</v>
+        <v>336.0</v>
       </c>
       <c r="H6" t="n">
-        <v>777.9615210634561</v>
+        <v>336.0</v>
       </c>
       <c r="I6" t="n">
-        <v>792.5545356471746</v>
+        <v>151.63750000000005</v>
       </c>
       <c r="J6" t="n">
-        <v>8121464.198030725</v>
+        <v>3020550.3899999997</v>
       </c>
       <c r="K6" t="n">
-        <v>47653871.62984403</v>
+        <v>5492700.0</v>
       </c>
       <c r="L6" t="n">
-        <v>39532407.43181331</v>
+        <v>2472149.6100000003</v>
       </c>
       <c r="M6" t="n">
-        <v>3.94</v>
+        <v>0.148</v>
       </c>
       <c r="N6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O6" t="n">
-        <v>4.287</v>
+        <v>0.155</v>
       </c>
       <c r="P6" t="n">
-        <v>0.347</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c s="2" r="A7" t="n">
-        <v>40946.729166666664</v>
+        <v>40942.229166666664</v>
       </c>
       <c r="B7" t="n">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="n">
+        <v>122.00886716059162</v>
+      </c>
+      <c r="E7" t="n">
+        <v>18.034000000000002</v>
+      </c>
+      <c r="F7" t="n">
+        <v>18</v>
+      </c>
+      <c r="G7" t="n">
+        <v>675.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>675.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>334.98080000000004</v>
+      </c>
+      <c r="J7" t="n">
+        <v>13974745.230000004</v>
+      </c>
+      <c r="K7" t="n">
+        <v>26066700.0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>12091954.769999996</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2.076</v>
+      </c>
+      <c r="N7" t="n">
         <v>6</v>
       </c>
-      <c r="D7" t="n">
-        <v>58.5240850612532</v>
-      </c>
-      <c r="E7" t="n">
-        <v>4.571999999999999</v>
-      </c>
-      <c r="F7" t="n">
-        <v>4</v>
-      </c>
-      <c r="G7" t="n">
-        <v>211.5527382949428</v>
-      </c>
-      <c r="H7" t="n">
-        <v>211.5527382949428</v>
-      </c>
-      <c r="I7" t="n">
-        <v>179.7291314583274</v>
-      </c>
-      <c r="J7" t="n">
-        <v>126987.66694647353</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1527394.4788524425</v>
-      </c>
-      <c r="L7" t="n">
-        <v>1400406.811905969</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.059</v>
-      </c>
-      <c r="N7" t="n">
-        <v>7</v>
-      </c>
       <c r="O7" t="n">
-        <v>0.063</v>
+        <v>2.143</v>
       </c>
       <c r="P7" t="n">
-        <v>0.004</v>
+        <v>0.067</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c s="2" r="A8" t="n">
-        <v>40977.25</v>
+        <v>40944.416666666664</v>
       </c>
       <c r="B8" t="n">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C8" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>225.7912434773228</v>
+        <v>136.1969361926139</v>
       </c>
       <c r="E8" t="n">
-        <v>18.034</v>
+        <v>19.050000000000004</v>
       </c>
       <c r="F8" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G8" t="n">
-        <v>404.6357610214328</v>
+        <v>551.0</v>
       </c>
       <c r="H8" t="n">
-        <v>404.6357610214328</v>
+        <v>551.0</v>
       </c>
       <c r="I8" t="n">
-        <v>583.509408218148</v>
+        <v>260.0941</v>
       </c>
       <c r="J8" t="n">
-        <v>-1385003.0848929444</v>
+        <v>9687786.894</v>
       </c>
       <c r="K8" t="n">
-        <v>5162423.677055798</v>
+        <v>17671500.0</v>
       </c>
       <c r="L8" t="n">
-        <v>6547426.761948742</v>
+        <v>7983713.106000001</v>
       </c>
       <c r="M8" t="n">
-        <v>0.992</v>
+        <v>0.933</v>
       </c>
       <c r="N8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O8" t="n">
-        <v>1.122</v>
+        <v>0.977</v>
       </c>
       <c r="P8" t="n">
-        <v>0.13</v>
+        <v>0.043</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c s="2" r="A9" t="n">
-        <v>40984.520833333336</v>
+        <v>40944.958333333336</v>
       </c>
       <c r="B9" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C9" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D9" t="n">
-        <v>54.731793144969465</v>
+        <v>166.85405181863675</v>
       </c>
       <c r="E9" t="n">
-        <v>8.889999999999999</v>
+        <v>83.05800000000002</v>
       </c>
       <c r="F9" t="n">
+        <v>83</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1470.9999999999998</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1470.9999999999998</v>
+      </c>
+      <c r="I9" t="n">
+        <v>776.5541000000001</v>
+      </c>
+      <c r="J9" t="n">
+        <v>53436013.47000001</v>
+      </c>
+      <c r="K9" t="n">
+        <v>102293100.0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>48857086.52999999</v>
+      </c>
+      <c r="M9" t="n">
+        <v>8.029</v>
+      </c>
+      <c r="N9" t="n">
         <v>8</v>
       </c>
-      <c r="G9" t="n">
-        <v>207.5257116858246</v>
-      </c>
-      <c r="H9" t="n">
-        <v>207.5257116858246</v>
-      </c>
-      <c r="I9" t="n">
-        <v>206.77703686895904</v>
-      </c>
-      <c r="J9" t="n">
-        <v>1662.6713568111882</v>
-      </c>
-      <c r="K9" t="n">
-        <v>2595742.037175725</v>
-      </c>
-      <c r="L9" t="n">
-        <v>2594079.365818914</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.255</v>
-      </c>
-      <c r="N9" t="n">
-        <v>9</v>
-      </c>
       <c r="O9" t="n">
-        <v>0.283</v>
+        <v>8.417</v>
       </c>
       <c r="P9" t="n">
-        <v>0.028</v>
+        <v>0.388</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c s="2" r="A10" t="n">
-        <v>40985.489583333336</v>
+        <v>40976.6875</v>
       </c>
       <c r="B10" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>381.16477418259853</v>
+        <v>404.41707844863413</v>
       </c>
       <c r="E10" t="n">
-        <v>30.987999999999992</v>
+        <v>23.875999999999998</v>
       </c>
       <c r="F10" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G10" t="n">
-        <v>361.9635596523701</v>
+        <v>616.0</v>
       </c>
       <c r="H10" t="n">
-        <v>361.9635596523701</v>
+        <v>616.0</v>
       </c>
       <c r="I10" t="n">
-        <v>241.84269490258072</v>
+        <v>280.75250000000005</v>
       </c>
       <c r="J10" t="n">
-        <v>1090637.4593928596</v>
+        <v>2201135.49</v>
       </c>
       <c r="K10" t="n">
-        <v>5335480.600166548</v>
+        <v>5751900.0</v>
       </c>
       <c r="L10" t="n">
-        <v>4244843.140773688</v>
+        <v>3550764.51</v>
       </c>
       <c r="M10" t="n">
-        <v>1.547</v>
+        <v>2.771</v>
       </c>
       <c r="N10" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O10" t="n">
-        <v>1.603</v>
+        <v>2.826</v>
       </c>
       <c r="P10" t="n">
         <v>0.055</v>
@@ -956,698 +956,698 @@
     </row>
     <row r="11" spans="1:16">
       <c s="2" r="A11" t="n">
-        <v>40989.84375</v>
+        <v>40977.25</v>
       </c>
       <c r="B11" t="n">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C11" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D11" t="n">
-        <v>170.3107428674363</v>
+        <v>206.90395688039456</v>
       </c>
       <c r="E11" t="n">
-        <v>14.985999999999999</v>
+        <v>18.034</v>
       </c>
       <c r="F11" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G11" t="n">
-        <v>279.72963499016237</v>
+        <v>861.0</v>
       </c>
       <c r="H11" t="n">
-        <v>279.72963499016237</v>
+        <v>861.0</v>
       </c>
       <c r="I11" t="n">
-        <v>251.41631411575463</v>
+        <v>590.6285</v>
       </c>
       <c r="J11" t="n">
-        <v>486997.8884443296</v>
+        <v>5461073.819999998</v>
       </c>
       <c r="K11" t="n">
-        <v>6007486.885110861</v>
+        <v>14332500.0</v>
       </c>
       <c r="L11" t="n">
-        <v>5520488.996666531</v>
+        <v>8871426.180000002</v>
       </c>
       <c r="M11" t="n">
-        <v>0.645</v>
+        <v>2.464</v>
       </c>
       <c r="N11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O11" t="n">
-        <v>0.758</v>
+        <v>2.611</v>
       </c>
       <c r="P11" t="n">
-        <v>0.113</v>
+        <v>0.147</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c s="2" r="A12" t="n">
-        <v>40990.21875</v>
+        <v>40984.416666666664</v>
       </c>
       <c r="B12" t="n">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="C12" t="n">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>157.51162489718936</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0</v>
+        <v>22.606</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G12" t="n">
-        <v>203.52704348531333</v>
+        <v>442.0</v>
       </c>
       <c r="H12" t="n">
-        <v>203.52704348531333</v>
+        <v>442.0</v>
       </c>
       <c r="I12" t="n">
-        <v>211.37394461281983</v>
+        <v>229.1065</v>
       </c>
       <c r="J12" t="n">
-        <v>-65940.07848783978</v>
+        <v>4553236.98</v>
       </c>
       <c r="K12" t="n">
-        <v>1517094.1574945762</v>
+        <v>8804700.0</v>
       </c>
       <c r="L12" t="n">
-        <v>1583034.235982416</v>
+        <v>4251463.02</v>
       </c>
       <c r="M12" t="n">
-        <v>0.057</v>
+        <v>1.467</v>
       </c>
       <c r="N12" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O12" t="n">
-        <v>0.072</v>
+        <v>1.51</v>
       </c>
       <c r="P12" t="n">
-        <v>0.015</v>
+        <v>0.043</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c s="2" r="A13" t="n">
-        <v>40990.90625</v>
+        <v>40985.489583333336</v>
       </c>
       <c r="B13" t="n">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C13" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>392.19297050657303</v>
+        <v>381.16477418259853</v>
       </c>
       <c r="E13" t="n">
-        <v>35.306000000000004</v>
+        <v>30.987999999999992</v>
       </c>
       <c r="F13" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G13" t="n">
-        <v>679.5636452953319</v>
+        <v>670.0</v>
       </c>
       <c r="H13" t="n">
-        <v>679.5636452953319</v>
+        <v>670.0</v>
       </c>
       <c r="I13" t="n">
-        <v>655.489375696788</v>
+        <v>254.9295</v>
       </c>
       <c r="J13" t="n">
-        <v>1873747.4868929796</v>
+        <v>5159530.17</v>
       </c>
       <c r="K13" t="n">
-        <v>11390355.997047016</v>
+        <v>9700200.0</v>
       </c>
       <c r="L13" t="n">
-        <v>9516608.510154037</v>
+        <v>4540669.83</v>
       </c>
       <c r="M13" t="n">
-        <v>2.695</v>
+        <v>2.88</v>
       </c>
       <c r="N13" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O13" t="n">
-        <v>2.98</v>
+        <v>2.939</v>
       </c>
       <c r="P13" t="n">
-        <v>0.284</v>
+        <v>0.059</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c s="2" r="A14" t="n">
-        <v>40993.145833333336</v>
+        <v>40989.84375</v>
       </c>
       <c r="B14" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C14" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D14" t="n">
-        <v>319.4904634178281</v>
+        <v>170.3107428674363</v>
       </c>
       <c r="E14" t="n">
-        <v>49.53</v>
+        <v>14.985999999999999</v>
       </c>
       <c r="F14" t="n">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="G14" t="n">
-        <v>817.3422884940093</v>
+        <v>516.0</v>
       </c>
       <c r="H14" t="n">
-        <v>817.3422884940093</v>
+        <v>516.0</v>
       </c>
       <c r="I14" t="n">
-        <v>1006.032168284175</v>
+        <v>280.75250000000005</v>
       </c>
       <c r="J14" t="n">
-        <v>-289966.01257101446</v>
+        <v>5031134.999999997</v>
       </c>
       <c r="K14" t="n">
-        <v>23663785.09361779</v>
+        <v>10868400.0</v>
       </c>
       <c r="L14" t="n">
-        <v>23953751.106188804</v>
+        <v>5837265.000000003</v>
       </c>
       <c r="M14" t="n">
-        <v>4.743</v>
+        <v>1.258</v>
       </c>
       <c r="N14" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O14" t="n">
-        <v>5.296</v>
+        <v>1.379</v>
       </c>
       <c r="P14" t="n">
-        <v>0.552</v>
+        <v>0.121</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c s="2" r="A15" t="n">
-        <v>41037.197916666664</v>
+        <v>40990.21875</v>
       </c>
       <c r="B15" t="n">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C15" t="n">
-        <v>4</v>
-      </c>
-      <c r="D15" t="n">
-        <v>367.3603538096914</v>
+        <v>11</v>
       </c>
       <c r="E15" t="n">
-        <v>25.654000000000003</v>
+        <v>0.0</v>
       </c>
       <c r="F15" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>340.08321600151805</v>
+        <v>366.0</v>
       </c>
       <c r="H15" t="n">
-        <v>340.08321600151805</v>
+        <v>366.0</v>
       </c>
       <c r="I15" t="n">
-        <v>354.4683425700709</v>
+        <v>229.1065</v>
       </c>
       <c r="J15" t="n">
-        <v>184806.8863221868</v>
+        <v>1023122.2500000005</v>
       </c>
       <c r="K15" t="n">
-        <v>2738571.6547077466</v>
+        <v>2716200.0</v>
       </c>
       <c r="L15" t="n">
-        <v>2553764.76838556</v>
+        <v>1693077.7499999995</v>
       </c>
       <c r="M15" t="n">
-        <v>1.82</v>
+        <v>0.113</v>
       </c>
       <c r="N15" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O15" t="n">
-        <v>1.903</v>
+        <v>0.128</v>
       </c>
       <c r="P15" t="n">
-        <v>0.083</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c s="2" r="A16" t="n">
-        <v>41051.8125</v>
+        <v>40990.90625</v>
       </c>
       <c r="B16" t="n">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C16" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D16" t="n">
-        <v>211.35322195810247</v>
+        <v>382.53642017912205</v>
       </c>
       <c r="E16" t="n">
-        <v>27.178</v>
+        <v>35.306000000000004</v>
       </c>
       <c r="F16" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="G16" t="n">
-        <v>932.72540995223</v>
+        <v>1281.9999999999998</v>
       </c>
       <c r="H16" t="n">
-        <v>932.72540995223</v>
+        <v>1281.9999999999998</v>
       </c>
       <c r="I16" t="n">
-        <v>1050.1827069920002</v>
+        <v>642.2745000000001</v>
       </c>
       <c r="J16" t="n">
-        <v>-1210072.8869409394</v>
+        <v>11498172.750000006</v>
       </c>
       <c r="K16" t="n">
-        <v>10287623.390817473</v>
+        <v>21906900.0</v>
       </c>
       <c r="L16" t="n">
-        <v>11497696.277758412</v>
+        <v>10408727.249999994</v>
       </c>
       <c r="M16" t="n">
-        <v>3.21</v>
+        <v>5.346</v>
       </c>
       <c r="N16" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O16" t="n">
-        <v>3.627</v>
+        <v>5.636</v>
       </c>
       <c r="P16" t="n">
-        <v>0.418</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="17" spans="1:16">
       <c s="2" r="A17" t="n">
-        <v>41052.333333333336</v>
+        <v>40993.145833333336</v>
       </c>
       <c r="B17" t="n">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="C17" t="n">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="D17" t="n">
-        <v>295.84935706761945</v>
+        <v>315.9027222930877</v>
       </c>
       <c r="E17" t="n">
-        <v>88.90000000000009</v>
+        <v>49.53</v>
       </c>
       <c r="F17" t="n">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="G17" t="n">
-        <v>1703.889894439881</v>
+        <v>1546.0</v>
       </c>
       <c r="H17" t="n">
-        <v>1703.889894439881</v>
+        <v>1546.0</v>
       </c>
       <c r="I17" t="n">
-        <v>2539.026304779525</v>
+        <v>926.3275</v>
       </c>
       <c r="J17" t="n">
-        <v>-22397035.53037475</v>
+        <v>19284902.99999999</v>
       </c>
       <c r="K17" t="n">
-        <v>57564474.58662528</v>
+        <v>44687700.0</v>
       </c>
       <c r="L17" t="n">
-        <v>79961510.11700003</v>
+        <v>25402797.00000001</v>
       </c>
       <c r="M17" t="n">
-        <v>1.262</v>
+        <v>9.432</v>
       </c>
       <c r="N17" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O17" t="n">
-        <v>3.482</v>
+        <v>9.99</v>
       </c>
       <c r="P17" t="n">
-        <v>2.22</v>
+        <v>0.558</v>
       </c>
     </row>
     <row r="18" spans="1:16">
       <c s="2" r="A18" t="n">
-        <v>41339.375</v>
+        <v>41031.677083333336</v>
       </c>
       <c r="B18" t="n">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C18" t="n">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>429.1256815986641</v>
       </c>
       <c r="E18" t="n">
-        <v>21.580000000000002</v>
+        <v>30.226</v>
       </c>
       <c r="F18" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G18" t="n">
-        <v>520.108135216388</v>
+        <v>758.0</v>
       </c>
       <c r="H18" t="n">
-        <v>520.108135216388</v>
+        <v>758.0</v>
       </c>
       <c r="I18" t="n">
-        <v>358.3976793518582</v>
+        <v>177.46049999999997</v>
       </c>
       <c r="J18" t="n">
-        <v>7153820.1064860085</v>
+        <v>2271931.65</v>
       </c>
       <c r="K18" t="n">
-        <v>15138162.551559893</v>
+        <v>3034800.0</v>
       </c>
       <c r="L18" t="n">
-        <v>7984342.445073885</v>
+        <v>762868.3500000001</v>
       </c>
       <c r="M18" t="n">
-        <v>0.407</v>
+        <v>4.162</v>
       </c>
       <c r="N18" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O18" t="n">
-        <v>0.465</v>
+        <v>4.177</v>
       </c>
       <c r="P18" t="n">
-        <v>0.057</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="19" spans="1:16">
       <c s="2" r="A19" t="n">
-        <v>41380.447916666664</v>
+        <v>41037.197916666664</v>
       </c>
       <c r="B19" t="n">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="C19" t="n">
-        <v>21</v>
+        <v>2</v>
+      </c>
+      <c r="D19" t="n">
+        <v>367.3603538096914</v>
       </c>
       <c r="E19" t="n">
-        <v>102.04000000000003</v>
+        <v>25.654000000000003</v>
       </c>
       <c r="F19" t="n">
-        <v>102</v>
+        <v>25</v>
       </c>
       <c r="G19" t="n">
-        <v>1484.1824822160804</v>
+        <v>615.0</v>
       </c>
       <c r="H19" t="n">
-        <v>1484.1824822160804</v>
+        <v>615.0</v>
       </c>
       <c r="I19" t="n">
-        <v>1581.2396641464977</v>
+        <v>384.04450000000014</v>
       </c>
       <c r="J19" t="n">
-        <v>27518049.7213848</v>
+        <v>2405888.4599999995</v>
       </c>
       <c r="K19" t="n">
-        <v>55680898.919615865</v>
+        <v>5372100.0</v>
       </c>
       <c r="L19" t="n">
-        <v>28162849.198231064</v>
+        <v>2966211.5400000005</v>
       </c>
       <c r="M19" t="n">
-        <v>2.511</v>
+        <v>3.453</v>
       </c>
       <c r="N19" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O19" t="n">
-        <v>3.179</v>
+        <v>3.544</v>
       </c>
       <c r="P19" t="n">
-        <v>0.668</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="20" spans="1:16">
       <c s="2" r="A20" t="n">
-        <v>41387.541666666664</v>
+        <v>41051.78125</v>
       </c>
       <c r="B20" t="n">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="C20" t="n">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="D20" t="n">
-        <v>456.78361008053724</v>
+        <v>217.13000059046055</v>
       </c>
       <c r="E20" t="n">
-        <v>85.85000000000002</v>
+        <v>33.782000000000004</v>
       </c>
       <c r="F20" t="n">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="G20" t="n">
-        <v>3399.333534716154</v>
+        <v>1767.0</v>
       </c>
       <c r="H20" t="n">
-        <v>3399.333534716154</v>
+        <v>1767.0</v>
       </c>
       <c r="I20" t="n">
-        <v>3281.3277552056734</v>
+        <v>952.1505000000001</v>
       </c>
       <c r="J20" t="n">
-        <v>13217510.416186832</v>
+        <v>8159480.099999996</v>
       </c>
       <c r="K20" t="n">
-        <v>63079452.89305422</v>
+        <v>20515500.0</v>
       </c>
       <c r="L20" t="n">
-        <v>49861942.476867385</v>
+        <v>12356019.900000004</v>
       </c>
       <c r="M20" t="n">
-        <v>6.763</v>
+        <v>7.531</v>
       </c>
       <c r="N20" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O20" t="n">
-        <v>12.363</v>
+        <v>7.95</v>
       </c>
       <c r="P20" t="n">
-        <v>5.6</v>
+        <v>0.419</v>
       </c>
     </row>
     <row r="21" spans="1:16">
       <c s="2" r="A21" t="n">
-        <v>41394.59375</v>
+        <v>41052.322916666664</v>
       </c>
       <c r="B21" t="n">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="C21" t="n">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="D21" t="n">
-        <v>304.1158518111377</v>
+        <v>293.5283969788771</v>
       </c>
       <c r="E21" t="n">
-        <v>112.50400000000005</v>
+        <v>88.90000000000009</v>
       </c>
       <c r="F21" t="n">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="G21" t="n">
-        <v>2566.312433742783</v>
+        <v>3213.0</v>
       </c>
       <c r="H21" t="n">
-        <v>2566.312433742783</v>
+        <v>3213.0</v>
       </c>
       <c r="I21" t="n">
-        <v>3004.435912808097</v>
+        <v>4660.645</v>
       </c>
       <c r="J21" t="n">
-        <v>12472497.388130695</v>
+        <v>5301360.000000015</v>
       </c>
       <c r="K21" t="n">
-        <v>79245169.25754689</v>
+        <v>109278000.0</v>
       </c>
       <c r="L21" t="n">
-        <v>66772671.86941619</v>
+        <v>103976639.99999999</v>
       </c>
       <c r="M21" t="n">
-        <v>4.402</v>
+        <v>3.071</v>
       </c>
       <c r="N21" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O21" t="n">
-        <v>4.785</v>
+        <v>6.457</v>
       </c>
       <c r="P21" t="n">
-        <v>0.383</v>
+        <v>3.387</v>
       </c>
     </row>
     <row r="22" spans="1:16">
       <c s="2" r="A22" t="n">
-        <v>41441.114583333336</v>
+        <v>41339.385416666664</v>
       </c>
       <c r="B22" t="n">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C22" t="n">
-        <v>18</v>
-      </c>
-      <c r="D22" t="n">
-        <v>214.17756727916927</v>
+        <v>7</v>
       </c>
       <c r="E22" t="n">
-        <v>30.987999999999996</v>
+        <v>21.580000000000002</v>
       </c>
       <c r="F22" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G22" t="n">
-        <v>537.049872189737</v>
+        <v>910.0</v>
       </c>
       <c r="H22" t="n">
-        <v>537.049872189737</v>
+        <v>910.0</v>
       </c>
       <c r="I22" t="n">
-        <v>422.6689268689101</v>
+        <v>371.13300000000004</v>
       </c>
       <c r="J22" t="n">
-        <v>5184420.799513532</v>
+        <v>17141699.88</v>
       </c>
       <c r="K22" t="n">
-        <v>13745171.882638745</v>
+        <v>24873300.0</v>
       </c>
       <c r="L22" t="n">
-        <v>8560751.083125213</v>
+        <v>7731600.120000002</v>
       </c>
       <c r="M22" t="n">
-        <v>0.452</v>
+        <v>0.723</v>
       </c>
       <c r="N22" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O22" t="n">
-        <v>0.555</v>
+        <v>0.779</v>
       </c>
       <c r="P22" t="n">
-        <v>0.102</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="23" spans="1:16">
       <c s="2" r="A23" t="n">
-        <v>41468.708333333336</v>
+        <v>41380.458333333336</v>
       </c>
       <c r="B23" t="n">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C23" t="n">
-        <v>50</v>
-      </c>
-      <c r="D23" t="n">
-        <v>222.08001535707467</v>
+        <v>13</v>
       </c>
       <c r="E23" t="n">
-        <v>16.255999999999997</v>
+        <v>53.29</v>
       </c>
       <c r="F23" t="n">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="G23" t="n">
-        <v>279.72963499016237</v>
+        <v>2245.0</v>
       </c>
       <c r="H23" t="n">
-        <v>279.72963499016237</v>
+        <v>2245.0</v>
       </c>
       <c r="I23" t="n">
-        <v>131.6769974122379</v>
+        <v>861.7700000000001</v>
       </c>
       <c r="J23" t="n">
-        <v>1374814.5636877918</v>
+        <v>21679519.5</v>
       </c>
       <c r="K23" t="n">
-        <v>2488300.143100958</v>
+        <v>31155300.0</v>
       </c>
       <c r="L23" t="n">
-        <v>1113485.579413166</v>
+        <v>9475780.499999998</v>
       </c>
       <c r="M23" t="n">
-        <v>0.006</v>
+        <v>3.426</v>
       </c>
       <c r="N23" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O23" t="n">
-        <v>0.01</v>
+        <v>3.953</v>
       </c>
       <c r="P23" t="n">
-        <v>0.005</v>
+        <v>0.528</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c s="2" r="A24" t="n">
-        <v>41684.625</v>
+        <v>41387.5625</v>
       </c>
       <c r="B24" t="n">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="C24" t="n">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="D24" t="n">
-        <v>211.18470463168936</v>
+        <v>524.2251682840218</v>
       </c>
       <c r="E24" t="n">
-        <v>18.288</v>
+        <v>83.56000000000003</v>
       </c>
       <c r="F24" t="n">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="G24" t="n">
-        <v>867.5600044108552</v>
+        <v>5754.0</v>
       </c>
       <c r="H24" t="n">
-        <v>867.5600044108552</v>
+        <v>5754.0</v>
       </c>
       <c r="I24" t="n">
-        <v>1286.609662556251</v>
+        <v>6286.654</v>
       </c>
       <c r="J24" t="n">
-        <v>-52427.29830216151</v>
+        <v>18811242.0</v>
       </c>
       <c r="K24" t="n">
-        <v>6551207.808762237</v>
+        <v>77974200.0</v>
       </c>
       <c r="L24" t="n">
-        <v>6603635.107064399</v>
+        <v>59162958.0</v>
       </c>
       <c r="M24" t="n">
-        <v>0.428</v>
+        <v>10.904</v>
       </c>
       <c r="N24" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O24" t="n">
-        <v>0.588</v>
+        <v>20.37</v>
       </c>
       <c r="P24" t="n">
-        <v>0.16</v>
+        <v>9.466</v>
       </c>
     </row>
     <row r="25" spans="1:16">
       <c s="2" r="A25" t="n">
-        <v>41690.46875</v>
+        <v>41394.625</v>
       </c>
       <c r="B25" t="n">
         <v>93</v>
@@ -1656,816 +1656,1116 @@
         <v>6</v>
       </c>
       <c r="D25" t="n">
-        <v>188.68861131126698</v>
+        <v>341.0232530753944</v>
       </c>
       <c r="E25" t="n">
-        <v>29.971999999999994</v>
+        <v>112.50400000000005</v>
       </c>
       <c r="F25" t="n">
-        <v>29</v>
+        <v>112</v>
       </c>
       <c r="G25" t="n">
-        <v>820.6560148321361</v>
+        <v>4300.0</v>
       </c>
       <c r="H25" t="n">
-        <v>820.6560148321361</v>
+        <v>4300.0</v>
       </c>
       <c r="I25" t="n">
-        <v>358.3976793518582</v>
+        <v>5695.378000000001</v>
       </c>
       <c r="J25" t="n">
-        <v>5542411.718310494</v>
+        <v>23372052.120000035</v>
       </c>
       <c r="K25" t="n">
-        <v>8858273.353704652</v>
+        <v>102510900.0</v>
       </c>
       <c r="L25" t="n">
-        <v>3315861.635394158</v>
+        <v>79138847.87999997</v>
       </c>
       <c r="M25" t="n">
-        <v>1.234</v>
+        <v>6.691</v>
       </c>
       <c r="N25" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O25" t="n">
-        <v>1.318</v>
+        <v>7.162</v>
       </c>
       <c r="P25" t="n">
-        <v>0.084</v>
+        <v>0.471</v>
       </c>
     </row>
     <row r="26" spans="1:16">
       <c s="2" r="A26" t="n">
-        <v>41691.479166666664</v>
+        <v>41441.135416666664</v>
       </c>
       <c r="B26" t="n">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C26" t="n">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D26" t="n">
-        <v>264.0102042737488</v>
+        <v>245.37334329583072</v>
       </c>
       <c r="E26" t="n">
-        <v>51.562000000000005</v>
+        <v>28.701999999999998</v>
       </c>
       <c r="F26" t="n">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="G26" t="n">
-        <v>1447.290516299777</v>
+        <v>709.0000000000001</v>
       </c>
       <c r="H26" t="n">
-        <v>1447.290516299777</v>
+        <v>709.0000000000001</v>
       </c>
       <c r="I26" t="n">
-        <v>1687.7750099916739</v>
+        <v>500.2480000000001</v>
       </c>
       <c r="J26" t="n">
-        <v>10489070.431000007</v>
+        <v>3824241.12</v>
       </c>
       <c r="K26" t="n">
-        <v>24608924.596617155</v>
+        <v>11345400.0</v>
       </c>
       <c r="L26" t="n">
-        <v>14119854.165617147</v>
+        <v>7521158.88</v>
       </c>
       <c r="M26" t="n">
-        <v>2.244</v>
+        <v>0.421</v>
       </c>
       <c r="N26" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O26" t="n">
-        <v>3.276</v>
+        <v>0.531</v>
       </c>
       <c r="P26" t="n">
-        <v>1.032</v>
+        <v>0.109</v>
       </c>
     </row>
     <row r="27" spans="1:16">
       <c s="2" r="A27" t="n">
-        <v>41695.885416666664</v>
+        <v>41684.614583333336</v>
       </c>
       <c r="B27" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C27" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" t="n">
-        <v>296.9759842737743</v>
+        <v>201.39435789365186</v>
       </c>
       <c r="E27" t="n">
-        <v>60.19799999999998</v>
+        <v>18.288</v>
       </c>
       <c r="F27" t="n">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="G27" t="n">
-        <v>1145.8305357672787</v>
+        <v>1725.0</v>
       </c>
       <c r="H27" t="n">
-        <v>1145.8305357672787</v>
+        <v>1725.0</v>
       </c>
       <c r="I27" t="n">
-        <v>984.1324907437174</v>
+        <v>1654.9920000000006</v>
       </c>
       <c r="J27" t="n">
-        <v>13947349.954735454</v>
+        <v>5909513.399999999</v>
       </c>
       <c r="K27" t="n">
-        <v>30649951.661978334</v>
+        <v>14096700.0</v>
       </c>
       <c r="L27" t="n">
-        <v>16702601.70724288</v>
+        <v>8187186.600000001</v>
       </c>
       <c r="M27" t="n">
-        <v>2.187</v>
+        <v>0.994</v>
       </c>
       <c r="N27" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O27" t="n">
-        <v>2.605</v>
+        <v>1.18</v>
       </c>
       <c r="P27" t="n">
-        <v>0.419</v>
+        <v>0.186</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c s="2" r="A28" t="n">
-        <v>41697.083333333336</v>
+        <v>41685.375</v>
       </c>
       <c r="B28" t="n">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="C28" t="n">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="D28" t="n">
-        <v>67.65551578393902</v>
+        <v>201.48018476665044</v>
       </c>
       <c r="E28" t="n">
-        <v>19.811999999999998</v>
+        <v>11.684</v>
       </c>
       <c r="F28" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G28" t="n">
-        <v>409.7695516956053</v>
+        <v>364.0</v>
       </c>
       <c r="H28" t="n">
-        <v>409.7695516956053</v>
+        <v>364.0</v>
       </c>
       <c r="I28" t="n">
-        <v>272.05767317589516</v>
+        <v>190.37199999999999</v>
       </c>
       <c r="J28" t="n">
-        <v>985225.6662331633</v>
+        <v>1451689.5599999996</v>
       </c>
       <c r="K28" t="n">
-        <v>9070597.283806283</v>
+        <v>2972700.0</v>
       </c>
       <c r="L28" t="n">
-        <v>8085371.61757312</v>
+        <v>1521010.4400000004</v>
       </c>
       <c r="M28" t="n">
-        <v>0.068</v>
+        <v>0.364</v>
       </c>
       <c r="N28" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O28" t="n">
-        <v>0.156</v>
+        <v>0.381</v>
       </c>
       <c r="P28" t="n">
-        <v>0.088</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="29" spans="1:16">
       <c s="2" r="A29" t="n">
-        <v>41697.677083333336</v>
+        <v>41688.760416666664</v>
       </c>
       <c r="B29" t="n">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C29" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>166.45613318083673</v>
+        <v>196.71299072274226</v>
       </c>
       <c r="E29" t="n">
-        <v>14.732</v>
+        <v>11.429999999999998</v>
       </c>
       <c r="F29" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G29" t="n">
-        <v>528.5541962522935</v>
+        <v>402.99999999999994</v>
       </c>
       <c r="H29" t="n">
-        <v>528.5541962522935</v>
+        <v>402.99999999999994</v>
       </c>
       <c r="I29" t="n">
-        <v>329.83235900440934</v>
+        <v>73.5872</v>
       </c>
       <c r="J29" t="n">
-        <v>1978163.1042375332</v>
+        <v>1688281.56</v>
       </c>
       <c r="K29" t="n">
-        <v>8375508.379396529</v>
+        <v>2173500.0</v>
       </c>
       <c r="L29" t="n">
-        <v>6397345.275158996</v>
+        <v>485218.4399999999</v>
       </c>
       <c r="M29" t="n">
-        <v>0.405</v>
+        <v>0.056</v>
       </c>
       <c r="N29" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O29" t="n">
-        <v>0.473</v>
+        <v>0.057</v>
       </c>
       <c r="P29" t="n">
-        <v>0.068</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="30" spans="1:16">
       <c s="2" r="A30" t="n">
-        <v>41927.53125</v>
+        <v>41690.46875</v>
       </c>
       <c r="B30" t="n">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C30" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D30" t="n">
-        <v>186.29244359931045</v>
+        <v>181.58532244046833</v>
       </c>
       <c r="E30" t="n">
-        <v>17.272000000000002</v>
+        <v>29.971999999999994</v>
       </c>
       <c r="F30" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="G30" t="n">
-        <v>430.5400686181124</v>
+        <v>1620.0</v>
       </c>
       <c r="H30" t="n">
-        <v>430.5400686181124</v>
+        <v>1620.0</v>
       </c>
       <c r="I30" t="n">
-        <v>226.4826685909736</v>
+        <v>422.779</v>
       </c>
       <c r="J30" t="n">
-        <v>2157082.825688182</v>
+        <v>14399120.879999999</v>
       </c>
       <c r="K30" t="n">
-        <v>4408087.605496053</v>
+        <v>18865800.0</v>
       </c>
       <c r="L30" t="n">
-        <v>2251004.7798078707</v>
+        <v>4466679.120000002</v>
       </c>
       <c r="M30" t="n">
-        <v>0.101</v>
+        <v>2.513</v>
       </c>
       <c r="N30" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O30" t="n">
-        <v>0.181</v>
+        <v>2.619</v>
       </c>
       <c r="P30" t="n">
-        <v>0.081</v>
+        <v>0.106</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c s="2" r="A31" t="n">
-        <v>41927.739583333336</v>
+        <v>41691.479166666664</v>
       </c>
       <c r="B31" t="n">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="C31" t="n">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="D31" t="n">
-        <v>168.34885796302487</v>
+        <v>257.1172250536837</v>
       </c>
       <c r="E31" t="n">
-        <v>17.525999999999996</v>
+        <v>51.562000000000005</v>
       </c>
       <c r="F31" t="n">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="G31" t="n">
-        <v>457.026973572824</v>
+        <v>2826.0</v>
       </c>
       <c r="H31" t="n">
-        <v>457.026973572824</v>
+        <v>2826.0</v>
       </c>
       <c r="I31" t="n">
-        <v>238.27621249463925</v>
+        <v>2738.998</v>
       </c>
       <c r="J31" t="n">
-        <v>4289531.300567574</v>
+        <v>32762163.779999986</v>
       </c>
       <c r="K31" t="n">
-        <v>9329134.568935001</v>
+        <v>51633000.0</v>
       </c>
       <c r="L31" t="n">
-        <v>5039603.268367427</v>
+        <v>18870836.220000014</v>
       </c>
       <c r="M31" t="n">
-        <v>0.04</v>
+        <v>5.167</v>
       </c>
       <c r="N31" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O31" t="n">
-        <v>0.179</v>
+        <v>6.501</v>
       </c>
       <c r="P31" t="n">
-        <v>0.139</v>
+        <v>1.335</v>
       </c>
     </row>
     <row r="32" spans="1:16">
       <c s="2" r="A32" t="n">
-        <v>41945.072916666664</v>
+        <v>41692.322916666664</v>
       </c>
       <c r="B32" t="n">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="C32" t="n">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="D32" t="n">
-        <v>86.28644068787793</v>
+        <v>3.110626716862608</v>
       </c>
       <c r="E32" t="n">
-        <v>22.352000000000004</v>
+        <v>0.254</v>
       </c>
       <c r="F32" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>438.4253996935176</v>
+        <v>327.0</v>
       </c>
       <c r="H32" t="n">
-        <v>438.4253996935176</v>
+        <v>327.0</v>
       </c>
       <c r="I32" t="n">
-        <v>291.8426685888395</v>
+        <v>164.549</v>
       </c>
       <c r="J32" t="n">
-        <v>2901168.535598412</v>
+        <v>1345815.9</v>
       </c>
       <c r="K32" t="n">
-        <v>7153662.278275641</v>
+        <v>2585700.0</v>
       </c>
       <c r="L32" t="n">
-        <v>4252493.7426772285</v>
+        <v>1239884.1</v>
       </c>
       <c r="M32" t="n">
-        <v>0.02</v>
+        <v>0.012</v>
       </c>
       <c r="N32" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O32" t="n">
-        <v>0.133</v>
+        <v>0.017</v>
       </c>
       <c r="P32" t="n">
-        <v>0.113</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="33" spans="1:16">
       <c s="2" r="A33" t="n">
-        <v>41946.71875</v>
+        <v>41694.229166666664</v>
       </c>
       <c r="B33" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D33" t="n">
-        <v>271.5676304031019</v>
+        <v>286.5287500936365</v>
       </c>
       <c r="E33" t="n">
-        <v>43.17999999999999</v>
+        <v>20.32</v>
       </c>
       <c r="F33" t="n">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="G33" t="n">
-        <v>1160.8519140025217</v>
+        <v>617.0</v>
       </c>
       <c r="H33" t="n">
-        <v>1160.8519140025217</v>
+        <v>617.0</v>
       </c>
       <c r="I33" t="n">
-        <v>1757.149938730621</v>
+        <v>267.841</v>
       </c>
       <c r="J33" t="n">
-        <v>-3106110.1320976093</v>
+        <v>1489565.3399999999</v>
       </c>
       <c r="K33" t="n">
-        <v>18609537.129933264</v>
+        <v>2787300.0</v>
       </c>
       <c r="L33" t="n">
-        <v>21715647.262030873</v>
+        <v>1297734.6600000001</v>
       </c>
       <c r="M33" t="n">
-        <v>0.936</v>
+        <v>0.061</v>
       </c>
       <c r="N33" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O33" t="n">
-        <v>1.675</v>
+        <v>0.112</v>
       </c>
       <c r="P33" t="n">
-        <v>0.74</v>
+        <v>0.051</v>
       </c>
     </row>
     <row r="34" spans="1:16">
       <c s="2" r="A34" t="n">
-        <v>41955.395833333336</v>
+        <v>41695.885416666664</v>
       </c>
       <c r="B34" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C34" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D34" t="n">
-        <v>13.102616334793796</v>
+        <v>287.6669943068481</v>
       </c>
       <c r="E34" t="n">
-        <v>1.524</v>
+        <v>60.45199999999998</v>
       </c>
       <c r="F34" t="n">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="G34" t="n">
-        <v>384.3383604663907</v>
+        <v>2231.9999999999995</v>
       </c>
       <c r="H34" t="n">
-        <v>384.3383604663907</v>
+        <v>2231.9999999999995</v>
       </c>
       <c r="I34" t="n">
-        <v>125.55598293520461</v>
+        <v>939.2390000000001</v>
       </c>
       <c r="J34" t="n">
-        <v>1522656.737766617</v>
+        <v>43191582.480000004</v>
       </c>
       <c r="K34" t="n">
-        <v>2417353.81623045</v>
+        <v>64715400.0</v>
       </c>
       <c r="L34" t="n">
-        <v>894697.0784638327</v>
+        <v>21523817.519999992</v>
       </c>
       <c r="M34" t="n">
-        <v>0.063</v>
+        <v>4.698</v>
       </c>
       <c r="N34" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O34" t="n">
-        <v>0.07</v>
+        <v>5.168</v>
       </c>
       <c r="P34" t="n">
-        <v>0.008</v>
+        <v>0.469</v>
       </c>
     </row>
     <row r="35" spans="1:16">
       <c s="2" r="A35" t="n">
-        <v>41965.8125</v>
+        <v>41697.083333333336</v>
       </c>
       <c r="B35" t="n">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C35" t="n">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D35" t="n">
-        <v>306.8677646555146</v>
+        <v>163.08699943866492</v>
       </c>
       <c r="E35" t="n">
-        <v>78.74</v>
+        <v>35.814</v>
       </c>
       <c r="F35" t="n">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="G35" t="n">
-        <v>1221.648717007398</v>
+        <v>1078.0</v>
       </c>
       <c r="H35" t="n">
-        <v>1221.648717007398</v>
+        <v>1078.0</v>
       </c>
       <c r="I35" t="n">
-        <v>1638.1005236170938</v>
+        <v>396.956</v>
       </c>
       <c r="J35" t="n">
-        <v>-8329264.8307091445</v>
+        <v>20130878.699999988</v>
       </c>
       <c r="K35" t="n">
-        <v>36740857.427309945</v>
+        <v>41267700.0</v>
       </c>
       <c r="L35" t="n">
-        <v>45070122.25801909</v>
+        <v>21136821.300000012</v>
       </c>
       <c r="M35" t="n">
-        <v>1.216</v>
+        <v>1.094</v>
       </c>
       <c r="N35" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="O35" t="n">
-        <v>1.775</v>
+        <v>1.302</v>
       </c>
       <c r="P35" t="n">
-        <v>0.56</v>
+        <v>0.208</v>
       </c>
     </row>
     <row r="36" spans="1:16">
       <c s="2" r="A36" t="n">
-        <v>41967.885416666664</v>
+        <v>41927.53125</v>
       </c>
       <c r="B36" t="n">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C36" t="n">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D36" t="n">
-        <v>200.49292057864182</v>
+        <v>198.39082469674628</v>
       </c>
       <c r="E36" t="n">
-        <v>20.065999999999995</v>
+        <v>17.272000000000002</v>
       </c>
       <c r="F36" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G36" t="n">
-        <v>574.432674239805</v>
+        <v>777.0</v>
       </c>
       <c r="H36" t="n">
-        <v>574.432674239805</v>
+        <v>777.0</v>
       </c>
       <c r="I36" t="n">
-        <v>327.26458946972247</v>
+        <v>267.841</v>
       </c>
       <c r="J36" t="n">
-        <v>1779856.9482419658</v>
+        <v>4694805.54</v>
       </c>
       <c r="K36" t="n">
-        <v>7448406.705124993</v>
+        <v>7409700.0</v>
       </c>
       <c r="L36" t="n">
-        <v>5668549.756883027</v>
+        <v>2714894.46</v>
       </c>
       <c r="M36" t="n">
-        <v>0.207</v>
+        <v>0.218</v>
       </c>
       <c r="N36" t="n">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="O36" t="n">
-        <v>0.246</v>
+        <v>0.317</v>
       </c>
       <c r="P36" t="n">
-        <v>0.039</v>
+        <v>0.099</v>
       </c>
     </row>
     <row r="37" spans="1:16">
       <c s="2" r="A37" t="n">
-        <v>41977.864583333336</v>
+        <v>41927.739583333336</v>
       </c>
       <c r="B37" t="n">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="C37" t="n">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D37" t="n">
-        <v>285.3138446588298</v>
+        <v>171.50955744051024</v>
       </c>
       <c r="E37" t="n">
-        <v>65.278</v>
+        <v>17.525999999999996</v>
       </c>
       <c r="F37" t="n">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="G37" t="n">
-        <v>534.212480619587</v>
+        <v>827.0000000000001</v>
       </c>
       <c r="H37" t="n">
-        <v>534.212480619587</v>
+        <v>827.0000000000001</v>
       </c>
       <c r="I37" t="n">
-        <v>257.44575123281686</v>
+        <v>293.664</v>
       </c>
       <c r="J37" t="n">
-        <v>9887504.545242203</v>
+        <v>9649831.86</v>
       </c>
       <c r="K37" t="n">
-        <v>21341682.808284648</v>
+        <v>15527700.0</v>
       </c>
       <c r="L37" t="n">
-        <v>11454178.263042444</v>
+        <v>5877868.140000001</v>
       </c>
       <c r="M37" t="n">
-        <v>0.34</v>
+        <v>0.136</v>
       </c>
       <c r="N37" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="O37" t="n">
-        <v>0.521</v>
+        <v>0.305</v>
       </c>
       <c r="P37" t="n">
-        <v>0.181</v>
+        <v>0.169</v>
       </c>
     </row>
     <row r="38" spans="1:16">
       <c s="2" r="A38" t="n">
-        <v>41982.4375</v>
+        <v>41945.145833333336</v>
       </c>
       <c r="B38" t="n">
+        <v>35</v>
+      </c>
+      <c r="C38" t="n">
+        <v>64</v>
+      </c>
+      <c r="D38" t="n">
+        <v>85.36592353742058</v>
+      </c>
+      <c r="E38" t="n">
+        <v>16.001999999999995</v>
+      </c>
+      <c r="F38" t="n">
         <v>16</v>
       </c>
-      <c r="C38" t="n">
-        <v>83</v>
-      </c>
-      <c r="D38" t="n">
-        <v>475.241792054697</v>
-      </c>
-      <c r="E38" t="n">
-        <v>33.02</v>
-      </c>
-      <c r="F38" t="n">
-        <v>33</v>
-      </c>
       <c r="G38" t="n">
-        <v>2486.2900723944445</v>
+        <v>777.0</v>
       </c>
       <c r="H38" t="n">
-        <v>2486.2900723944445</v>
+        <v>777.0</v>
       </c>
       <c r="I38" t="n">
-        <v>2418.9295144547687</v>
+        <v>345.31000000000006</v>
       </c>
       <c r="J38" t="n">
-        <v>-9446271.740478741</v>
+        <v>5930668.08</v>
       </c>
       <c r="K38" t="n">
-        <v>14834248.003262656</v>
+        <v>9854100.0</v>
       </c>
       <c r="L38" t="n">
-        <v>24280519.743741397</v>
+        <v>3923431.9200000004</v>
       </c>
       <c r="M38" t="n">
-        <v>0.36</v>
+        <v>0.061</v>
       </c>
       <c r="N38" t="n">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="O38" t="n">
-        <v>2.125</v>
+        <v>0.174</v>
       </c>
       <c r="P38" t="n">
-        <v>1.765</v>
+        <v>0.113</v>
       </c>
     </row>
     <row r="39" spans="1:16">
       <c s="2" r="A39" t="n">
-        <v>41992.020833333336</v>
+        <v>41946.71875</v>
       </c>
       <c r="B39" t="n">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="C39" t="n">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="D39" t="n">
-        <v>285.23230520476153</v>
+        <v>278.2160273509692</v>
       </c>
       <c r="E39" t="n">
-        <v>60.19799999999999</v>
+        <v>43.17999999999999</v>
       </c>
       <c r="F39" t="n">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="G39" t="n">
-        <v>1240.879447169906</v>
+        <v>2184.0</v>
       </c>
       <c r="H39" t="n">
-        <v>1240.879447169906</v>
+        <v>2184.0</v>
       </c>
       <c r="I39" t="n">
-        <v>1562.396018052978</v>
+        <v>2936.0900000000006</v>
       </c>
       <c r="J39" t="n">
-        <v>-813824.8259628899</v>
+        <v>7073644.68</v>
       </c>
       <c r="K39" t="n">
-        <v>28147520.430733178</v>
+        <v>32589900.0</v>
       </c>
       <c r="L39" t="n">
-        <v>28961345.256696068</v>
+        <v>25516255.32</v>
       </c>
       <c r="M39" t="n">
-        <v>0.399</v>
+        <v>2.186</v>
       </c>
       <c r="N39" t="n">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="O39" t="n">
-        <v>1.236</v>
+        <v>3.05</v>
       </c>
       <c r="P39" t="n">
-        <v>0.837</v>
+        <v>0.864</v>
       </c>
     </row>
     <row r="40" spans="1:16">
       <c s="2" r="A40" t="n">
+        <v>41955.395833333336</v>
+      </c>
+      <c r="B40" t="n">
+        <v>92</v>
+      </c>
+      <c r="C40" t="n">
+        <v>7</v>
+      </c>
+      <c r="D40" t="n">
+        <v>13.102616334793796</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1.524</v>
+      </c>
+      <c r="F40" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" t="n">
+        <v>679.0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>679.0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>164.549</v>
+      </c>
+      <c r="J40" t="n">
+        <v>2610915.3</v>
+      </c>
+      <c r="K40" t="n">
+        <v>3588300.0</v>
+      </c>
+      <c r="L40" t="n">
+        <v>977384.7</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="N40" t="n">
+        <v>40</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="P40" t="n">
+        <v>0.008</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c s="2" r="A41" t="n">
+        <v>41965.8125</v>
+      </c>
+      <c r="B41" t="n">
+        <v>79</v>
+      </c>
+      <c r="C41" t="n">
+        <v>20</v>
+      </c>
+      <c r="D41" t="n">
+        <v>306.8677646555146</v>
+      </c>
+      <c r="E41" t="n">
+        <v>78.74</v>
+      </c>
+      <c r="F41" t="n">
+        <v>78</v>
+      </c>
+      <c r="G41" t="n">
+        <v>2255.0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>2255.0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>2640.4520000000007</v>
+      </c>
+      <c r="J41" t="n">
+        <v>16730345.340000026</v>
+      </c>
+      <c r="K41" t="n">
+        <v>65700900.0</v>
+      </c>
+      <c r="L41" t="n">
+        <v>48970554.659999974</v>
+      </c>
+      <c r="M41" t="n">
+        <v>2.544</v>
+      </c>
+      <c r="N41" t="n">
+        <v>45</v>
+      </c>
+      <c r="O41" t="n">
+        <v>3.215</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0.671</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c s="2" r="A42" t="n">
+        <v>41967.885416666664</v>
+      </c>
+      <c r="B42" t="n">
+        <v>88</v>
+      </c>
+      <c r="C42" t="n">
+        <v>11</v>
+      </c>
+      <c r="D42" t="n">
+        <v>200.49292057864182</v>
+      </c>
+      <c r="E42" t="n">
+        <v>20.065999999999995</v>
+      </c>
+      <c r="F42" t="n">
+        <v>20</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1040.0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1040.0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>371.13300000000004</v>
+      </c>
+      <c r="J42" t="n">
+        <v>5772572.819999998</v>
+      </c>
+      <c r="K42" t="n">
+        <v>12341700.0</v>
+      </c>
+      <c r="L42" t="n">
+        <v>6569127.180000002</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0.368</v>
+      </c>
+      <c r="N42" t="n">
+        <v>46</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0.414</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0.046</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c s="2" r="A43" t="n">
+        <v>41977.84375</v>
+      </c>
+      <c r="B43" t="n">
+        <v>81</v>
+      </c>
+      <c r="C43" t="n">
+        <v>18</v>
+      </c>
+      <c r="D43" t="n">
+        <v>274.0549097343187</v>
+      </c>
+      <c r="E43" t="n">
+        <v>65.278</v>
+      </c>
+      <c r="F43" t="n">
+        <v>65</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1192.0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>1192.0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>319.48699999999997</v>
+      </c>
+      <c r="J43" t="n">
+        <v>36460564.199999996</v>
+      </c>
+      <c r="K43" t="n">
+        <v>52292700.0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>15832135.800000003</v>
+      </c>
+      <c r="M43" t="n">
+        <v>1.036</v>
+      </c>
+      <c r="N43" t="n">
+        <v>47</v>
+      </c>
+      <c r="O43" t="n">
+        <v>1.268</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0.232</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c s="2" r="A44" t="n">
+        <v>41982.427083333336</v>
+      </c>
+      <c r="B44" t="n">
+        <v>48</v>
+      </c>
+      <c r="C44" t="n">
+        <v>51</v>
+      </c>
+      <c r="D44" t="n">
+        <v>437.76187532306676</v>
+      </c>
+      <c r="E44" t="n">
+        <v>34.797999999999995</v>
+      </c>
+      <c r="F44" t="n">
+        <v>34</v>
+      </c>
+      <c r="G44" t="n">
+        <v>4927.0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>4927.0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>4512.826000000001</v>
+      </c>
+      <c r="J44" t="n">
+        <v>4722626.700000018</v>
+      </c>
+      <c r="K44" t="n">
+        <v>39253500.0</v>
+      </c>
+      <c r="L44" t="n">
+        <v>34530873.29999998</v>
+      </c>
+      <c r="M44" t="n">
+        <v>2.426</v>
+      </c>
+      <c r="N44" t="n">
+        <v>48</v>
+      </c>
+      <c r="O44" t="n">
+        <v>5.021</v>
+      </c>
+      <c r="P44" t="n">
+        <v>2.595</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c s="2" r="A45" t="n">
+        <v>41992.010416666664</v>
+      </c>
+      <c r="B45" t="n">
+        <v>59</v>
+      </c>
+      <c r="C45" t="n">
+        <v>40</v>
+      </c>
+      <c r="D45" t="n">
+        <v>284.6076764001334</v>
+      </c>
+      <c r="E45" t="n">
+        <v>62.48399999999999</v>
+      </c>
+      <c r="F45" t="n">
+        <v>62</v>
+      </c>
+      <c r="G45" t="n">
+        <v>2598.0000000000005</v>
+      </c>
+      <c r="H45" t="n">
+        <v>2598.0000000000005</v>
+      </c>
+      <c r="I45" t="n">
+        <v>2443.36</v>
+      </c>
+      <c r="J45" t="n">
+        <v>20464599.599999983</v>
+      </c>
+      <c r="K45" t="n">
+        <v>53721000.0</v>
+      </c>
+      <c r="L45" t="n">
+        <v>33256400.400000017</v>
+      </c>
+      <c r="M45" t="n">
+        <v>1.439</v>
+      </c>
+      <c r="N45" t="n">
+        <v>49</v>
+      </c>
+      <c r="O45" t="n">
+        <v>2.408</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0.969</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c s="2" r="A46" t="n">
         <v>41994.020833333336</v>
       </c>
-      <c r="B40" t="n">
-        <v>43</v>
-      </c>
-      <c r="C40" t="n">
-        <v>56</v>
-      </c>
-      <c r="D40" t="n">
+      <c r="B46" t="n">
+        <v>63</v>
+      </c>
+      <c r="C46" t="n">
+        <v>36</v>
+      </c>
+      <c r="D46" t="n">
         <v>260.5078552965765</v>
       </c>
-      <c r="E40" t="n">
+      <c r="E46" t="n">
         <v>143.51000000000005</v>
       </c>
-      <c r="F40" t="n">
+      <c r="F46" t="n">
         <v>143</v>
       </c>
-      <c r="G40" t="n">
-        <v>1857.9208007783168</v>
-      </c>
-      <c r="H40" t="n">
-        <v>1857.9208007783168</v>
-      </c>
-      <c r="I40" t="n">
-        <v>2041.2999212915388</v>
-      </c>
-      <c r="J40" t="n">
-        <v>16680038.13672702</v>
-      </c>
-      <c r="K40" t="n">
-        <v>92698335.2245315</v>
-      </c>
-      <c r="L40" t="n">
-        <v>76018297.08780448</v>
-      </c>
-      <c r="M40" t="n">
-        <v>1.375</v>
-      </c>
-      <c r="N40" t="n">
-        <v>45</v>
-      </c>
-      <c r="O40" t="n">
-        <v>3.126</v>
-      </c>
-      <c r="P40" t="n">
-        <v>1.751</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16">
-      <c s="1" r="A41" t="s"/>
-      <c r="B41" t="n">
-        <v>72.5</v>
-      </c>
-      <c r="C41" t="n">
-        <v>26.9</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="G46" t="n">
+        <v>3497.0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>3497.0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>3625.9120000000007</v>
+      </c>
+      <c r="J46" t="n">
+        <v>83355909.84000003</v>
+      </c>
+      <c r="K46" t="n">
+        <v>174342600.0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>90986690.15999997</v>
+      </c>
+      <c r="M46" t="n">
+        <v>3.714</v>
+      </c>
+      <c r="N46" t="n">
+        <v>50</v>
+      </c>
+      <c r="O46" t="n">
+        <v>5.89</v>
+      </c>
+      <c r="P46" t="n">
+        <v>2.176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c s="1" r="A47" t="s"/>
+      <c r="B47" t="n">
+        <v>81.6</v>
+      </c>
+      <c r="C47" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="F47" t="s">
         <v>7</v>
       </c>
-      <c r="M41" t="s">
+      <c r="M47" t="s">
         <v>7</v>
       </c>
-      <c r="N41" t="s">
+      <c r="N47" t="s">
         <v>7</v>
       </c>
-      <c r="O41" t="s">
+      <c r="O47" t="s">
         <v>12</v>
       </c>
-      <c r="P41" t="s">
+      <c r="P47" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>